<commit_message>
Update formulas documentation and add new practice examples
</commit_message>
<xml_diff>
--- a/excel_files/formula_examples.xlsx
+++ b/excel_files/formula_examples.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DV\Assignment\Excel Basics\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E3C7F6BD-4457-45A3-9F14-42C9C7BBCF97}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83697C2-8972-4F82-A165-A8B8D4110A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF_example" sheetId="1" r:id="rId1"/>
     <sheet name="IFS_example" sheetId="3" r:id="rId2"/>
+    <sheet name="AND_example" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="35">
   <si>
     <t>Student Name</t>
   </si>
@@ -99,6 +113,33 @@
   </si>
   <si>
     <t>Marks(Out of 100)</t>
+  </si>
+  <si>
+    <t>Student_Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Assignment Status</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Not Submitted</t>
+  </si>
+  <si>
+    <t>Eligible for Trip</t>
+  </si>
+  <si>
+    <t>Attendance in %</t>
+  </si>
+  <si>
+    <t>Certificate Awarded or Not</t>
   </si>
 </sst>
 </file>
@@ -173,7 +214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -195,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,9 +276,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,26 +311,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,26 +346,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,7 +525,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C2" sqref="C2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,7 +589,7 @@
         <v>Pass</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:F16" si="1">IF(B3:B17&gt;75,"Elligible","Not Elligible")</f>
+        <f t="shared" ref="E3:E16" si="1">IF(B3:B17&gt;75,"Elligible","Not Elligible")</f>
         <v>Not Elligible</v>
       </c>
     </row>
@@ -842,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72578E1-E378-4B2D-8E0C-35DB37E44804}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -885,7 +892,7 @@
         <v>F</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.IFS(B2&gt;=85,"Excellent",B2&gt;=70,"Good",B2&gt;=50,"Average",B2&lt;50,"Need Improvement")</f>
+        <f t="shared" ref="E2:E16" si="0">_xlfn.IFS(B2&gt;=85,"Excellent",B2&gt;=70,"Good",B2&gt;=50,"Average",B2&lt;50,"Need Improvement")</f>
         <v>Need Improvement</v>
       </c>
     </row>
@@ -900,11 +907,11 @@
         <v>18</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D16" si="0">_xlfn.IFS(B3&gt;=90,"A",B3&gt;=75,"B",B3&gt;=60,"C",B3&gt;=50,"D",B3&lt;50,"F")</f>
+        <f t="shared" ref="D3:D16" si="1">_xlfn.IFS(B3&gt;=90,"A",B3&gt;=75,"B",B3&gt;=60,"C",B3&gt;=50,"D",B3&lt;50,"F")</f>
         <v>D</v>
       </c>
       <c r="E3" t="str">
-        <f>_xlfn.IFS(B3&gt;=85,"Excellent",B3&gt;=70,"Good",B3&gt;=50,"Average",B3&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Average</v>
       </c>
     </row>
@@ -919,11 +926,11 @@
         <v>18</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>C</v>
       </c>
       <c r="E4" t="str">
-        <f>_xlfn.IFS(B4&gt;=85,"Excellent",B4&gt;=70,"Good",B4&gt;=50,"Average",B4&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Good</v>
       </c>
     </row>
@@ -938,11 +945,11 @@
         <v>18</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>B</v>
       </c>
       <c r="E5" t="str">
-        <f>_xlfn.IFS(B5&gt;=85,"Excellent",B5&gt;=70,"Good",B5&gt;=50,"Average",B5&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Excellent</v>
       </c>
     </row>
@@ -957,11 +964,11 @@
         <v>18</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="E6" t="str">
-        <f>_xlfn.IFS(B6&gt;=85,"Excellent",B6&gt;=70,"Good",B6&gt;=50,"Average",B6&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Need Improvement</v>
       </c>
     </row>
@@ -976,11 +983,11 @@
         <v>18</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>B</v>
       </c>
       <c r="E7" t="str">
-        <f>_xlfn.IFS(B7&gt;=85,"Excellent",B7&gt;=70,"Good",B7&gt;=50,"Average",B7&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Excellent</v>
       </c>
     </row>
@@ -995,11 +1002,11 @@
         <v>19</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>C</v>
       </c>
       <c r="E8" t="str">
-        <f>_xlfn.IFS(B8&gt;=85,"Excellent",B8&gt;=70,"Good",B8&gt;=50,"Average",B8&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Average</v>
       </c>
     </row>
@@ -1014,11 +1021,11 @@
         <v>19</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>D</v>
       </c>
       <c r="E9" t="str">
-        <f>_xlfn.IFS(B9&gt;=85,"Excellent",B9&gt;=70,"Good",B9&gt;=50,"Average",B9&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Average</v>
       </c>
     </row>
@@ -1033,11 +1040,11 @@
         <v>18</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>B</v>
       </c>
       <c r="E10" t="str">
-        <f>_xlfn.IFS(B10&gt;=85,"Excellent",B10&gt;=70,"Good",B10&gt;=50,"Average",B10&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Good</v>
       </c>
     </row>
@@ -1052,11 +1059,11 @@
         <v>19</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="E11" t="str">
-        <f>_xlfn.IFS(B11&gt;=85,"Excellent",B11&gt;=70,"Good",B11&gt;=50,"Average",B11&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Need Improvement</v>
       </c>
     </row>
@@ -1071,11 +1078,11 @@
         <v>19</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>B</v>
       </c>
       <c r="E12" t="str">
-        <f>_xlfn.IFS(B12&gt;=85,"Excellent",B12&gt;=70,"Good",B12&gt;=50,"Average",B12&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Good</v>
       </c>
     </row>
@@ -1090,11 +1097,11 @@
         <v>18</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="E13" t="str">
-        <f>_xlfn.IFS(B13&gt;=85,"Excellent",B13&gt;=70,"Good",B13&gt;=50,"Average",B13&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Need Improvement</v>
       </c>
     </row>
@@ -1109,11 +1116,11 @@
         <v>18</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="E14" t="str">
-        <f>_xlfn.IFS(B14&gt;=85,"Excellent",B14&gt;=70,"Good",B14&gt;=50,"Average",B14&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Need Improvement</v>
       </c>
     </row>
@@ -1128,11 +1135,11 @@
         <v>19</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>D</v>
       </c>
       <c r="E15" t="str">
-        <f>_xlfn.IFS(B15&gt;=85,"Excellent",B15&gt;=70,"Good",B15&gt;=50,"Average",B15&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Average</v>
       </c>
     </row>
@@ -1147,12 +1154,481 @@
         <v>19</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>B</v>
       </c>
       <c r="E16" t="str">
-        <f>_xlfn.IFS(B16&gt;=85,"Excellent",B16&gt;=70,"Good",B16&gt;=50,"Average",B16&lt;50,"Need Improvement")</f>
+        <f t="shared" si="0"/>
         <v>Good</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D7C345-F1BB-41A8-A479-B001C22CE572}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="23.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(AND(D2&gt;=50,F2="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(AND(D2&gt;=60,E2&gt;=75),"Certificate Awarded","Not Awarded")</f>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(AND(D3&gt;=50,F3="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H16" si="0">IF(AND(D3&gt;=60,E3&gt;=75),"Certificate Awarded","Not Awarded")</f>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(AND(D4&gt;=50,F4="Submitted"),"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>Certificate Awarded</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="str">
+        <f>IF(AND(D5&gt;=50,F5="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="str">
+        <f>IF(AND(D6&gt;=50,F6="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="str">
+        <f>IF(AND(D7&gt;=50,F7="Submitted"),"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>Certificate Awarded</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="str">
+        <f>IF(AND(D8&gt;=50,F8="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>Certificate Awarded</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="str">
+        <f>IF(AND(D9&gt;=50,F9="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="str">
+        <f>IF(AND(D10&gt;=50,F10="Submitted"),"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="str">
+        <f>IF(AND(D11&gt;=50,F11="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="str">
+        <f>IF(AND(D12&gt;=50,F12="Submitted"),"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>Certificate Awarded</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="str">
+        <f>IF(AND(D13&gt;=50,F13="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="str">
+        <f>IF(AND(D14&gt;=50,F14="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="str">
+        <f>IF(AND(D15&gt;=50,F15="Submitted"),"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Awarded</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="str">
+        <f>IF(AND(D16&gt;=50,F16="Submitted"),"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>Certificate Awarded</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add OR and SUM function documentation with examples and images
</commit_message>
<xml_diff>
--- a/excel_files/formula_examples.xlsx
+++ b/excel_files/formula_examples.xlsx
@@ -8,34 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DV\Assignment\Excel Basics\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83697C2-8972-4F82-A165-A8B8D4110A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB80AD9-FF71-4F86-83D1-7903183E8320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF_example" sheetId="1" r:id="rId1"/>
     <sheet name="IFS_example" sheetId="3" r:id="rId2"/>
     <sheet name="AND_example" sheetId="4" r:id="rId3"/>
+    <sheet name="OR_example" sheetId="5" r:id="rId4"/>
+    <sheet name="SUM_example" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="41">
   <si>
     <t>Student Name</t>
   </si>
@@ -140,6 +129,24 @@
   </si>
   <si>
     <t>Certificate Awarded or Not</t>
+  </si>
+  <si>
+    <t>Extra Credit</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Hindi Marks (out of 100)</t>
+  </si>
+  <si>
+    <t>English Marks (out of 100)</t>
+  </si>
+  <si>
+    <t>Maths Marks (out of 100)</t>
+  </si>
+  <si>
+    <t>Total Marks</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D7C345-F1BB-41A8-A479-B001C22CE572}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1231,7 +1238,7 @@
         <v>30</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(AND(D2&gt;=50,F2="Submitted"),"Yes","No")</f>
+        <f t="shared" ref="G2:G16" si="0">IF(AND(D2&gt;=50,F2="Submitted"),"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="H2" t="str">
@@ -1259,11 +1266,11 @@
         <v>31</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(AND(D3&gt;=50,F3="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H16" si="0">IF(AND(D3&gt;=60,E3&gt;=75),"Certificate Awarded","Not Awarded")</f>
+        <f t="shared" ref="H3:H16" si="1">IF(AND(D3&gt;=60,E3&gt;=75),"Certificate Awarded","Not Awarded")</f>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1287,11 +1294,11 @@
         <v>30</v>
       </c>
       <c r="G4" t="str">
-        <f>IF(AND(D4&gt;=50,F4="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Certificate Awarded</v>
       </c>
     </row>
@@ -1315,11 +1322,11 @@
         <v>31</v>
       </c>
       <c r="G5" t="str">
-        <f>IF(AND(D5&gt;=50,F5="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1343,11 +1350,11 @@
         <v>31</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(AND(D6&gt;=50,F6="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1371,11 +1378,11 @@
         <v>30</v>
       </c>
       <c r="G7" t="str">
-        <f>IF(AND(D7&gt;=50,F7="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Certificate Awarded</v>
       </c>
     </row>
@@ -1399,11 +1406,11 @@
         <v>31</v>
       </c>
       <c r="G8" t="str">
-        <f>IF(AND(D8&gt;=50,F8="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Certificate Awarded</v>
       </c>
     </row>
@@ -1427,11 +1434,11 @@
         <v>31</v>
       </c>
       <c r="G9" t="str">
-        <f>IF(AND(D9&gt;=50,F9="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1455,11 +1462,11 @@
         <v>30</v>
       </c>
       <c r="G10" t="str">
-        <f>IF(AND(D10&gt;=50,F10="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1483,11 +1490,11 @@
         <v>31</v>
       </c>
       <c r="G11" t="str">
-        <f>IF(AND(D11&gt;=50,F11="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1511,11 +1518,11 @@
         <v>30</v>
       </c>
       <c r="G12" t="str">
-        <f>IF(AND(D12&gt;=50,F12="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Certificate Awarded</v>
       </c>
     </row>
@@ -1539,11 +1546,11 @@
         <v>30</v>
       </c>
       <c r="G13" t="str">
-        <f>IF(AND(D13&gt;=50,F13="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1567,11 +1574,11 @@
         <v>31</v>
       </c>
       <c r="G14" t="str">
-        <f>IF(AND(D14&gt;=50,F14="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1595,11 +1602,11 @@
         <v>31</v>
       </c>
       <c r="G15" t="str">
-        <f>IF(AND(D15&gt;=50,F15="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Not Awarded</v>
       </c>
     </row>
@@ -1623,11 +1630,11 @@
         <v>30</v>
       </c>
       <c r="G16" t="str">
-        <f>IF(AND(D16&gt;=50,F16="Submitted"),"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Certificate Awarded</v>
       </c>
     </row>
@@ -1635,4 +1642,882 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C791FB1A-90D4-436A-8DB8-93316C16172E}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(OR(D2&gt;=80,F2="Submitted"),"Extra Credit","No Credit")</f>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(OR(D2&lt;40,E2&lt;60),"Warning","Ok")</f>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G16" si="0">IF(OR(D3&gt;=80,F3="Submitted"),"Extra Credit","No Credit")</f>
+        <v>No Credit</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H16" si="1">IF(OR(D3&lt;40,E3&lt;60),"Warning","Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>No Credit</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>No Credit</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>No Credit</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>No Credit</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>No Credit</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>Warning</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>No Credit</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>Extra Credit</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988B176C-6834-4C56-ACF7-03F7A0903D12}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="26.7265625" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="G2">
+        <f>SUM(D2,E2,F2)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G16" si="0">SUM(D3,E3,F3)</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>67</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>67</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="F16">
+        <v>98</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="3" t="str">
+        <f>"Total Marks = " &amp;SUM(G2:$G$16)</f>
+        <v>Total Marks = 2980</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new practice examples and images for COUNT, COUNTA, COUNTIF, COUNTIFS, and SUMIF functions
</commit_message>
<xml_diff>
--- a/excel_files/formula_examples.xlsx
+++ b/excel_files/formula_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DV\Assignment\Excel Basics\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB80AD9-FF71-4F86-83D1-7903183E8320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EDDB55-ED6E-454C-ACFB-CAB57D17E4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF_example" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,19 @@
     <sheet name="AND_example" sheetId="4" r:id="rId3"/>
     <sheet name="OR_example" sheetId="5" r:id="rId4"/>
     <sheet name="SUM_example" sheetId="6" r:id="rId5"/>
+    <sheet name="SUMIF_example" sheetId="7" r:id="rId6"/>
+    <sheet name="SUMIFS_example" sheetId="8" r:id="rId7"/>
+    <sheet name="COUNT_example" sheetId="9" r:id="rId8"/>
+    <sheet name="COUNTIF_example" sheetId="10" r:id="rId9"/>
+    <sheet name="COUNTIFS_example" sheetId="11" r:id="rId10"/>
+    <sheet name="COUNTA_example" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="51">
   <si>
     <t>Student Name</t>
   </si>
@@ -147,6 +153,36 @@
   </si>
   <si>
     <t>Total Marks</t>
+  </si>
+  <si>
+    <t>Sum based on Maths Marks</t>
+  </si>
+  <si>
+    <t>Science Marks (out of 100)</t>
+  </si>
+  <si>
+    <t>Sum Based on Science MARKS</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>10B</t>
+  </si>
+  <si>
+    <t>Practice 1</t>
+  </si>
+  <si>
+    <t>Practice 2</t>
+  </si>
+  <si>
+    <t>Parctice 1</t>
+  </si>
+  <si>
+    <t>Parctice 2</t>
   </si>
 </sst>
 </file>
@@ -852,6 +888,710 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F404C9DD-021D-40AC-9B20-8A86386AC711}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="23.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="G2">
+        <f>COUNTIFS($F$2:$F$16,"&gt;=50",$C$2:$C$16,"&gt;75")</f>
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIFS($E$2:$E$16,"&gt;=60",$B$2:$B$16,"10A")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="F16">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85208218-AA4F-4D91-83D4-27ADB6A26625}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="22.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA($A$2:$A$16)</f>
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <f>COUNTA($D$2:$D$16,$E$2:$E$16,$F$2:$F$16)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="F16">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72578E1-E378-4B2D-8E0C-35DB37E44804}">
   <dimension ref="A1:E16"/>
@@ -1180,7 +1920,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F16"/>
+      <selection activeCell="E1" sqref="E1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2115,8 +2855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988B176C-6834-4C56-ACF7-03F7A0903D12}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2520,4 +3260,1466 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93AD3C6-080B-4305-9D5E-44B434A971BA}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" customWidth="1"/>
+    <col min="8" max="8" width="24.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>78</v>
+      </c>
+      <c r="H2">
+        <f>SUMIF($G$1:$G$16,"&gt;=50",$G$1:$G$16)</f>
+        <v>977</v>
+      </c>
+      <c r="I2">
+        <f>SUMIF($D$2:$D$16,"&gt;=75",$F$2:$F$16)</f>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>90</v>
+      </c>
+      <c r="E4">
+        <v>72</v>
+      </c>
+      <c r="F4">
+        <v>78</v>
+      </c>
+      <c r="G4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>88</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
+      </c>
+      <c r="G5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="F6">
+        <v>45</v>
+      </c>
+      <c r="G6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>94</v>
+      </c>
+      <c r="E7">
+        <v>86</v>
+      </c>
+      <c r="F7">
+        <v>67</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>98</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="F8">
+        <v>80</v>
+      </c>
+      <c r="G8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>99</v>
+      </c>
+      <c r="E9">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>99</v>
+      </c>
+      <c r="G9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>82</v>
+      </c>
+      <c r="F10">
+        <v>89</v>
+      </c>
+      <c r="G10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>55</v>
+      </c>
+      <c r="E11">
+        <v>27</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+      <c r="G11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>82</v>
+      </c>
+      <c r="F12">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>56</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>56</v>
+      </c>
+      <c r="E14">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>58</v>
+      </c>
+      <c r="G14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>67</v>
+      </c>
+      <c r="E15">
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <v>98</v>
+      </c>
+      <c r="G15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>89</v>
+      </c>
+      <c r="E16">
+        <v>83</v>
+      </c>
+      <c r="F16">
+        <v>67</v>
+      </c>
+      <c r="G16">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BF4CBD-123F-482F-8352-2074C73BF73D}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="G2">
+        <f>SUMIFS($F$2:$F$16,$F$2:$F$16,"&gt;=50",$C$2:$C$16,"&gt;75")</f>
+        <v>552</v>
+      </c>
+      <c r="H2">
+        <f>SUMIFS($E$2:$E$16,$E$2:$E$16,"&gt;=60",$B$2:$B$16,"10A")</f>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="F16">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDF573C-D7BC-46AA-859B-12244055D56E}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="23.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="G2">
+        <f>COUNT($F$2:$F$16)</f>
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <f>COUNT($E$2:$E$16)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="F16">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D8AB8B-C354-4EE7-8441-B1D13E8D2116}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="21.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="G2">
+        <f>COUNTIF($F$2:$F$16,"&gt;=50")</f>
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIF($B$2:$B$16,"10A")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>67</v>
+      </c>
+      <c r="F16">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>